<commit_message>
My sprint info added
</commit_message>
<xml_diff>
--- a/Project/Phase 2/Sprint3/Burndown chart.xlsx
+++ b/Project/Phase 2/Sprint3/Burndown chart.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhertz/Documents/subjects/SE/deliver/ganttproject/Project/Phase 2/Sprint3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9288C3E-7D78-F648-A103-958419BE6EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{309438F3-8A0B-40E3-A1D2-AFC674DAE873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -24,6 +24,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,6 +34,9 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>Sprint 4 Burndown Chart</t>
+  </si>
   <si>
     <t>Task ID</t>
   </si>
@@ -45,28 +50,25 @@
     <t>Day 0</t>
   </si>
   <si>
-    <t>Remaining Effort</t>
+    <t>Debug the code to know how it works</t>
+  </si>
+  <si>
+    <t>Find and correct possible bugs (It had one)</t>
+  </si>
+  <si>
+    <t>See how to implement feature 1 (Ricardo) and 2 (James,Iago,Francisco,Joao)</t>
+  </si>
+  <si>
+    <t>Create a java program to encapsulate tasks so James can use in the ganttproject</t>
   </si>
   <si>
     <t>Completed Effort</t>
   </si>
   <si>
-    <t>Ideal Burndown</t>
+    <t>Remaining Effort</t>
   </si>
   <si>
-    <t>Implement feature 1</t>
-  </si>
-  <si>
-    <t>Implement feature 2</t>
-  </si>
-  <si>
-    <t>Upload sprints to github</t>
-  </si>
-  <si>
-    <t>Take metrics</t>
-  </si>
-  <si>
-    <t>Sprint 4 Burndown Chart</t>
+    <t>Ideal Burndown</t>
   </si>
 </sst>
 </file>
@@ -77,7 +79,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]d/mmm/yy;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,7 +164,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -289,41 +291,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -438,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -455,25 +422,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -485,13 +437,13 @@
     <xf numFmtId="165" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -507,31 +459,34 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -546,10 +501,10 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -577,7 +532,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="pt-PT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -639,7 +594,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -654,19 +609,11 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'Burndown Chart'!$B$10:$C$10</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Completed Effort</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Completed Effort</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4"/>
+              <a:srgbClr val="FFC000"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -684,32 +631,32 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-8D0E-4F8E-897D-5B1720B3868B}"/>
+              <c16:uniqueId val="{00000000-F629-4E15-B173-7FCE21FEFDEF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -733,15 +680,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'Burndown Chart'!$B$11:$C$11</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Remaining Effort</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Remaining Effort</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -806,13 +745,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>13</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3</c:v>
@@ -821,13 +760,13 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -835,7 +774,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8D0E-4F8E-897D-5B1720B3868B}"/>
+              <c16:uniqueId val="{00000001-F629-4E15-B173-7FCE21FEFDEF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -843,15 +782,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'Burndown Chart'!$B$12:$C$12</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Ideal Burndown</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Ideal Burndown</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -904,25 +835,25 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>13</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.142857142857142</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.2857142857142847</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.4285714285714288</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.5714285714285712</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.7142857142857135</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.8571428571428577</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -933,7 +864,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8D0E-4F8E-897D-5B1720B3868B}"/>
+              <c16:uniqueId val="{00000002-F629-4E15-B173-7FCE21FEFDEF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -991,7 +922,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1048433599"/>
@@ -1075,7 +1006,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1107,7 +1038,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1048432767"/>
@@ -1149,7 +1080,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1186,7 +1117,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1757,27 +1688,32 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>16807</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>180414</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>177054</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>640419</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>6165</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52BFCA64-3DDA-4711-BDFA-D2973C7C7C4B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E077733-FB04-4551-9EB0-2AC0E5129503}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{52BFCA64-3DDA-4711-BDFA-D2973C7C7C4B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1795,7 +1731,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2083,7 +2019,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2094,54 +2030,54 @@
   <dimension ref="B1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:12" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
+    <row r="1" spans="2:12" ht="15.95" thickBot="1"/>
+    <row r="2" spans="2:12" ht="27" thickBot="1">
+      <c r="B2" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
     </row>
-    <row r="3" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="30"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="32"/>
+    <row r="3" spans="2:12" ht="15.95" thickBot="1">
+      <c r="B3" s="26"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="28"/>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B4" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="33" t="s">
+    <row r="4" spans="2:12">
+      <c r="B4" s="31" t="s">
         <v>1</v>
       </c>
+      <c r="C4" s="29" t="s">
+        <v>2</v>
+      </c>
       <c r="D4" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" s="3">
         <v>44886</v>
@@ -2165,11 +2101,11 @@
         <v>44892</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="36"/>
-      <c r="C5" s="34"/>
+    <row r="5" spans="2:12" ht="15.95" thickBot="1">
+      <c r="B5" s="32"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5" s="4">
         <v>1</v>
@@ -2193,206 +2129,244 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="19">
+    <row r="6" spans="2:12">
+      <c r="B6" s="14">
         <v>1</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="17">
+        <v>3</v>
+      </c>
+      <c r="E6" s="5">
+        <v>1</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1</v>
+      </c>
+      <c r="G6" s="5">
+        <v>1</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0</v>
+      </c>
+      <c r="K6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
+      <c r="B7" s="16">
+        <v>2</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="18">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0</v>
+      </c>
+      <c r="K7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12">
+      <c r="B8" s="16">
+        <v>3</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="22">
-        <v>5</v>
-      </c>
-      <c r="E6" s="5">
+      <c r="D8" s="18">
         <v>2</v>
       </c>
-      <c r="F6" s="6">
-        <v>2</v>
-      </c>
-      <c r="G6" s="6">
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
         <v>1</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
+      <c r="I8" s="5">
+        <v>1</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0</v>
+      </c>
+      <c r="K8" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="21">
-        <v>2</v>
-      </c>
-      <c r="C7" s="20" t="s">
+    <row r="9" spans="2:12">
+      <c r="B9" s="16">
+        <v>4</v>
+      </c>
+      <c r="C9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="23">
-        <v>5</v>
-      </c>
-      <c r="E7" s="7">
+      <c r="D9" s="18">
         <v>1</v>
       </c>
-      <c r="F7" s="8">
-        <v>2</v>
-      </c>
-      <c r="G7" s="8">
-        <v>2</v>
-      </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="K9" s="5">
+        <v>0.5</v>
+      </c>
     </row>
-    <row r="8" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="21">
-        <v>3</v>
-      </c>
-      <c r="C8" s="20" t="s">
+    <row r="10" spans="2:12">
+      <c r="B10" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="23">
-        <v>2</v>
-      </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8">
-        <v>1</v>
-      </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-    </row>
-    <row r="9" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="21">
-        <v>4</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="23">
-        <v>1</v>
-      </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8">
-        <v>0</v>
-      </c>
-      <c r="I9" s="8">
-        <v>0</v>
-      </c>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="27"/>
+      <c r="C10" s="23"/>
       <c r="D10" s="1">
         <v>0</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="7">
         <f t="shared" ref="E10:K10" si="0">SUM(E6:E9)</f>
-        <v>3</v>
-      </c>
-      <c r="F10" s="12">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G10" s="12">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H10" s="12">
+        <v>1</v>
+      </c>
+      <c r="F10" s="7">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I10" s="12">
+      <c r="G10" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="12">
+        <v>2</v>
+      </c>
+      <c r="H10" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K10" s="12">
+        <v>1</v>
+      </c>
+      <c r="I10" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L10" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="J10" s="7">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="L10" s="13"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="14">
+    <row r="11" spans="2:12">
+      <c r="B11" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="34"/>
+      <c r="D11" s="9">
         <f>SUM(D6:D10)</f>
-        <v>13</v>
-      </c>
-      <c r="E11" s="15">
+        <v>7</v>
+      </c>
+      <c r="E11" s="10">
         <f t="shared" ref="E11:K11" si="1">D11-SUM(E6:E9)</f>
-        <v>10</v>
-      </c>
-      <c r="F11" s="13">
+        <v>6</v>
+      </c>
+      <c r="F11" s="8">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="G11" s="13">
+        <v>5</v>
+      </c>
+      <c r="G11" s="8">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H11" s="8">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11" s="8">
         <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J11" s="6">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="K11" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="15.95" thickBot="1">
+      <c r="B12" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="21"/>
+      <c r="D12" s="11">
+        <f>D11</f>
+        <v>7</v>
+      </c>
+      <c r="E12" s="12">
+        <f t="shared" ref="E12:K12" si="2">$D$12-($D$12/$K$5*E5)</f>
+        <v>6</v>
+      </c>
+      <c r="F12" s="12">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G12" s="12">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="H12" s="12">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="I12" s="12">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="J11" s="11">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="K11" s="11">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="16">
-        <f>D11</f>
-        <v>13</v>
-      </c>
-      <c r="E12" s="17">
-        <f t="shared" ref="E12:K12" si="2">$D$12-($D$12/$K$5*E5)</f>
-        <v>11.142857142857142</v>
-      </c>
-      <c r="F12" s="17">
+      <c r="J12" s="12">
         <f t="shared" si="2"/>
-        <v>9.2857142857142847</v>
-      </c>
-      <c r="G12" s="17">
-        <f t="shared" si="2"/>
-        <v>7.4285714285714288</v>
-      </c>
-      <c r="H12" s="17">
-        <f t="shared" si="2"/>
-        <v>5.5714285714285712</v>
-      </c>
-      <c r="I12" s="17">
-        <f t="shared" si="2"/>
-        <v>3.7142857142857135</v>
-      </c>
-      <c r="J12" s="17">
-        <f t="shared" si="2"/>
-        <v>1.8571428571428577</v>
-      </c>
-      <c r="K12" s="17">
+        <v>1</v>
+      </c>
+      <c r="K12" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>

</xml_diff>